<commit_message>
[Pipette] Femto에 전달할 MP Data update Main, Transformer PCB
</commit_message>
<xml_diff>
--- a/Femto Project 비용 List.xlsx
+++ b/Femto Project 비용 List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="1890" windowWidth="28800" windowHeight="12060" activeTab="2"/>
+    <workbookView xWindow="3735" yWindow="1890" windowWidth="28800" windowHeight="12060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="전체 비용 List" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="489">
   <si>
     <t>Vendor</t>
   </si>
@@ -1850,6 +1850,14 @@
   </si>
   <si>
     <t>Artwork</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>V2.0</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -4298,6 +4306,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4331,27 +4342,36 @@
     <xf numFmtId="0" fontId="31" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="33" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4364,15 +4384,6 @@
     <xf numFmtId="0" fontId="31" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="31" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4386,9 +4397,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5396,29 +5404,29 @@
       </c>
     </row>
     <row r="9" spans="2:16" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="451" t="s">
+      <c r="C9" s="452" t="s">
         <v>296</v>
       </c>
-      <c r="D9" s="452"/>
-      <c r="E9" s="452"/>
+      <c r="D9" s="453"/>
+      <c r="E9" s="453"/>
       <c r="F9" s="264">
         <f>SUM(F6:F8)</f>
         <v>138411</v>
       </c>
-      <c r="H9" s="451" t="s">
+      <c r="H9" s="452" t="s">
         <v>296</v>
       </c>
-      <c r="I9" s="452"/>
-      <c r="J9" s="452"/>
+      <c r="I9" s="453"/>
+      <c r="J9" s="453"/>
       <c r="K9" s="264">
         <f>SUM(K6:K8)</f>
         <v>42250</v>
       </c>
-      <c r="M9" s="451" t="s">
+      <c r="M9" s="452" t="s">
         <v>296</v>
       </c>
-      <c r="N9" s="452"/>
-      <c r="O9" s="452"/>
+      <c r="N9" s="453"/>
+      <c r="O9" s="453"/>
       <c r="P9" s="264">
         <f>SUM(P6:P8)</f>
         <v>44750</v>
@@ -5559,37 +5567,37 @@
       </c>
     </row>
     <row r="14" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="451" t="s">
+      <c r="C14" s="452" t="s">
         <v>299</v>
       </c>
-      <c r="D14" s="452"/>
-      <c r="E14" s="472">
+      <c r="D14" s="453"/>
+      <c r="E14" s="473">
         <f>F12</f>
         <v>553644</v>
       </c>
-      <c r="F14" s="473"/>
-      <c r="H14" s="451" t="s">
+      <c r="F14" s="474"/>
+      <c r="H14" s="452" t="s">
         <v>299</v>
       </c>
-      <c r="I14" s="452"/>
-      <c r="J14" s="472">
+      <c r="I14" s="453"/>
+      <c r="J14" s="473">
         <f>K12</f>
         <v>169000</v>
       </c>
-      <c r="K14" s="473"/>
-      <c r="M14" s="451" t="s">
+      <c r="K14" s="474"/>
+      <c r="M14" s="452" t="s">
         <v>299</v>
       </c>
-      <c r="N14" s="452"/>
-      <c r="O14" s="472">
+      <c r="N14" s="453"/>
+      <c r="O14" s="473">
         <f>P12</f>
         <v>150000</v>
       </c>
-      <c r="P14" s="473"/>
+      <c r="P14" s="474"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C15" s="474"/>
-      <c r="D15" s="474"/>
+      <c r="C15" s="475"/>
+      <c r="D15" s="475"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
@@ -5713,11 +5721,11 @@
       </c>
     </row>
     <row r="22" spans="3:16" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="451" t="s">
+      <c r="C22" s="452" t="s">
         <v>296</v>
       </c>
-      <c r="D22" s="452"/>
-      <c r="E22" s="452"/>
+      <c r="D22" s="453"/>
+      <c r="E22" s="453"/>
       <c r="F22" s="264">
         <f>SUM(F19:F21)</f>
         <v>45292</v>
@@ -5740,11 +5748,11 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="M23" s="451" t="s">
+      <c r="M23" s="452" t="s">
         <v>296</v>
       </c>
-      <c r="N23" s="452"/>
-      <c r="O23" s="452"/>
+      <c r="N23" s="453"/>
+      <c r="O23" s="453"/>
       <c r="P23" s="264">
         <f>SUM(P20:P22)</f>
         <v>18000</v>
@@ -5854,24 +5862,24 @@
       </c>
     </row>
     <row r="28" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="451" t="s">
+      <c r="C28" s="452" t="s">
         <v>299</v>
       </c>
-      <c r="D28" s="452"/>
-      <c r="E28" s="472">
+      <c r="D28" s="453"/>
+      <c r="E28" s="473">
         <f>SUM(F25:F27)</f>
         <v>291168</v>
       </c>
-      <c r="F28" s="473"/>
-      <c r="M28" s="451" t="s">
+      <c r="F28" s="474"/>
+      <c r="M28" s="452" t="s">
         <v>299</v>
       </c>
-      <c r="N28" s="452"/>
-      <c r="O28" s="472">
+      <c r="N28" s="453"/>
+      <c r="O28" s="473">
         <f>P26</f>
         <v>90000</v>
       </c>
-      <c r="P28" s="473"/>
+      <c r="P28" s="474"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.3">
       <c r="M31" s="56" t="s">
@@ -5949,11 +5957,11 @@
       </c>
     </row>
     <row r="37" spans="13:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M37" s="451" t="s">
+      <c r="M37" s="452" t="s">
         <v>296</v>
       </c>
-      <c r="N37" s="452"/>
-      <c r="O37" s="452"/>
+      <c r="N37" s="453"/>
+      <c r="O37" s="453"/>
       <c r="P37" s="264">
         <f>SUM(P34:P36)</f>
         <v>13500</v>
@@ -6010,18 +6018,29 @@
       </c>
     </row>
     <row r="42" spans="13:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M42" s="451" t="s">
+      <c r="M42" s="452" t="s">
         <v>299</v>
       </c>
-      <c r="N42" s="452"/>
-      <c r="O42" s="472">
+      <c r="N42" s="453"/>
+      <c r="O42" s="473">
         <f>P40</f>
         <v>13500</v>
       </c>
-      <c r="P42" s="473"/>
+      <c r="P42" s="474"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="H9:J9"/>
@@ -6030,17 +6049,6 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7047,8 +7055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7099,22 +7107,22 @@
       <c r="I4" s="261" t="s">
         <v>373</v>
       </c>
-      <c r="K4" s="453" t="s">
+      <c r="K4" s="454" t="s">
         <v>94</v>
       </c>
-      <c r="L4" s="447"/>
-      <c r="M4" s="455" t="s">
+      <c r="L4" s="448"/>
+      <c r="M4" s="456" t="s">
         <v>84</v>
       </c>
-      <c r="N4" s="455"/>
-      <c r="O4" s="455"/>
-      <c r="P4" s="447" t="s">
+      <c r="N4" s="456"/>
+      <c r="O4" s="456"/>
+      <c r="P4" s="448" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="447" t="s">
+      <c r="Q4" s="448" t="s">
         <v>89</v>
       </c>
-      <c r="R4" s="449" t="s">
+      <c r="R4" s="450" t="s">
         <v>92</v>
       </c>
     </row>
@@ -7144,8 +7152,8 @@
         <f t="shared" ref="I5:I10" si="0">G5*H5</f>
         <v>750000</v>
       </c>
-      <c r="K5" s="454"/>
-      <c r="L5" s="448"/>
+      <c r="K5" s="455"/>
+      <c r="L5" s="449"/>
       <c r="M5" s="385" t="s">
         <v>85</v>
       </c>
@@ -7155,9 +7163,9 @@
       <c r="O5" s="385" t="s">
         <v>96</v>
       </c>
-      <c r="P5" s="448"/>
-      <c r="Q5" s="448"/>
-      <c r="R5" s="450"/>
+      <c r="P5" s="449"/>
+      <c r="Q5" s="449"/>
+      <c r="R5" s="451"/>
     </row>
     <row r="6" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="203">
@@ -7185,10 +7193,10 @@
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="K6" s="451" t="s">
+      <c r="K6" s="452" t="s">
         <v>97</v>
       </c>
-      <c r="L6" s="452"/>
+      <c r="L6" s="453"/>
       <c r="M6" s="141">
         <v>1</v>
       </c>
@@ -7237,10 +7245,10 @@
         <f t="shared" si="0"/>
         <v>750000</v>
       </c>
-      <c r="K7" s="445" t="s">
+      <c r="K7" s="446" t="s">
         <v>486</v>
       </c>
-      <c r="L7" s="446"/>
+      <c r="L7" s="447"/>
       <c r="M7" s="141"/>
       <c r="N7" s="104">
         <v>1</v>
@@ -7473,7 +7481,7 @@
         <v>250000</v>
       </c>
       <c r="I15" s="444">
-        <f t="shared" ref="I15:I16" si="3">G15*H15</f>
+        <f t="shared" ref="I15:I17" si="3">G15*H15</f>
         <v>375000</v>
       </c>
     </row>
@@ -7505,14 +7513,31 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="203"/>
-      <c r="C17" s="347"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="86"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="347"/>
-      <c r="H17" s="347"/>
-      <c r="I17" s="18"/>
+      <c r="B17" s="203">
+        <v>43317</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="D17" s="86" t="s">
+        <v>487</v>
+      </c>
+      <c r="E17" s="86" t="s">
+        <v>488</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>372</v>
+      </c>
+      <c r="G17" s="347">
+        <v>2</v>
+      </c>
+      <c r="H17" s="9">
+        <v>250000</v>
+      </c>
+      <c r="I17" s="444">
+        <f t="shared" si="3"/>
+        <v>500000</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="203"/>
@@ -7604,8 +7629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7631,31 +7656,31 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="453" t="s">
+      <c r="B3" s="454" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="447"/>
-      <c r="D3" s="455" t="s">
+      <c r="C3" s="448"/>
+      <c r="D3" s="456" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="455"/>
-      <c r="F3" s="455"/>
-      <c r="G3" s="447" t="s">
+      <c r="E3" s="456"/>
+      <c r="F3" s="456"/>
+      <c r="G3" s="448" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="447" t="s">
+      <c r="H3" s="448" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="465" t="s">
+      <c r="I3" s="469" t="s">
         <v>92</v>
       </c>
-      <c r="J3" s="463" t="s">
+      <c r="J3" s="467" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="4" spans="2:15" s="137" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="469"/>
-      <c r="C4" s="467"/>
+      <c r="B4" s="463"/>
+      <c r="C4" s="464"/>
       <c r="D4" s="384" t="s">
         <v>85</v>
       </c>
@@ -7665,13 +7690,13 @@
       <c r="F4" s="384" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="467"/>
-      <c r="H4" s="467"/>
-      <c r="I4" s="466"/>
-      <c r="J4" s="464"/>
+      <c r="G4" s="464"/>
+      <c r="H4" s="464"/>
+      <c r="I4" s="470"/>
+      <c r="J4" s="468"/>
     </row>
     <row r="5" spans="2:15" s="341" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="460" t="s">
+      <c r="B5" s="457" t="s">
         <v>357</v>
       </c>
       <c r="C5" s="363" t="s">
@@ -7703,7 +7728,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" s="137" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="462"/>
+      <c r="B6" s="459"/>
       <c r="C6" s="356" t="s">
         <v>359</v>
       </c>
@@ -7728,13 +7753,13 @@
         <f t="shared" si="2"/>
         <v>600000</v>
       </c>
-      <c r="J6" s="475">
+      <c r="J6" s="445">
         <f>I6</f>
         <v>600000</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="460" t="s">
+      <c r="B7" s="457" t="s">
         <v>93</v>
       </c>
       <c r="C7" s="139" t="s">
@@ -7776,7 +7801,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="461"/>
+      <c r="B8" s="462"/>
       <c r="C8" s="345" t="s">
         <v>90</v>
       </c>
@@ -7804,7 +7829,7 @@
       <c r="J8" s="361"/>
     </row>
     <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="462"/>
+      <c r="B9" s="459"/>
       <c r="C9" s="349" t="s">
         <v>91</v>
       </c>
@@ -7832,7 +7857,7 @@
       <c r="J9" s="362"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="460" t="s">
+      <c r="B10" s="457" t="s">
         <v>95</v>
       </c>
       <c r="C10" s="139" t="s">
@@ -7862,7 +7887,7 @@
       <c r="J10" s="360"/>
     </row>
     <row r="11" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="461"/>
+      <c r="B11" s="462"/>
       <c r="C11" s="345" t="s">
         <v>361</v>
       </c>
@@ -7890,7 +7915,7 @@
       <c r="J11" s="361"/>
     </row>
     <row r="12" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="461"/>
+      <c r="B12" s="462"/>
       <c r="C12" s="345" t="s">
         <v>362</v>
       </c>
@@ -7918,7 +7943,7 @@
       <c r="J12" s="361"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="461"/>
+      <c r="B13" s="462"/>
       <c r="C13" s="345" t="s">
         <v>90</v>
       </c>
@@ -7946,7 +7971,7 @@
       <c r="J13" s="361"/>
     </row>
     <row r="14" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="462"/>
+      <c r="B14" s="459"/>
       <c r="C14" s="349" t="s">
         <v>91</v>
       </c>
@@ -7991,28 +8016,28 @@
     </row>
     <row r="23" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="460" t="s">
+      <c r="B24" s="457" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="456"/>
-      <c r="D24" s="468" t="s">
+      <c r="C24" s="458"/>
+      <c r="D24" s="461" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="468"/>
-      <c r="F24" s="468"/>
-      <c r="G24" s="456" t="s">
+      <c r="E24" s="461"/>
+      <c r="F24" s="461"/>
+      <c r="G24" s="458" t="s">
         <v>88</v>
       </c>
-      <c r="H24" s="456" t="s">
+      <c r="H24" s="458" t="s">
         <v>89</v>
       </c>
-      <c r="I24" s="458" t="s">
+      <c r="I24" s="465" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="462"/>
-      <c r="C25" s="457"/>
+      <c r="B25" s="459"/>
+      <c r="C25" s="460"/>
       <c r="D25" s="138" t="s">
         <v>85</v>
       </c>
@@ -8022,15 +8047,15 @@
       <c r="F25" s="138" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="457"/>
-      <c r="H25" s="457"/>
-      <c r="I25" s="459"/>
+      <c r="G25" s="460"/>
+      <c r="H25" s="460"/>
+      <c r="I25" s="466"/>
     </row>
     <row r="26" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="451" t="s">
+      <c r="B26" s="452" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="452"/>
+      <c r="C26" s="453"/>
       <c r="D26" s="141">
         <v>3</v>
       </c>
@@ -8071,11 +8096,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B3:C4"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="I24:I25"/>
@@ -8086,6 +8106,11 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B3:C4"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12055,15 +12080,15 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="451" t="s">
+      <c r="C9" s="452" t="s">
         <v>346</v>
       </c>
-      <c r="D9" s="452"/>
-      <c r="E9" s="470">
+      <c r="D9" s="453"/>
+      <c r="E9" s="471">
         <f>SUM(F7:F8)</f>
         <v>620000</v>
       </c>
-      <c r="F9" s="471"/>
+      <c r="F9" s="472"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>